<commit_message>
specs: all versions cleanup
</commit_message>
<xml_diff>
--- a/v1/documentation/Specs_v1.xlsx
+++ b/v1/documentation/Specs_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victoriadudley\Desktop\Team-Infinite\v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>If both distances are the same, output first ID</t>
   </si>
@@ -74,12 +74,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>DEVELOPMENT TIME</t>
-  </si>
-  <si>
-    <t>TEST TIME</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -90,6 +84,15 @@
   </si>
   <si>
     <t>VERSION1</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT TIME (HRS)</t>
+  </si>
+  <si>
+    <t>TEST TIME (HRS)</t>
+  </si>
+  <si>
+    <t>STATUS</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -339,31 +342,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -374,7 +406,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -400,20 +432,23 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -699,21 +734,21 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD21"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="73.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="67.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -729,17 +764,17 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="24" t="s">
-        <v>19</v>
+      <c r="C2" s="21" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -747,35 +782,37 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -789,9 +826,9 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -805,9 +842,9 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -821,9 +858,9 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -837,9 +874,9 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -853,9 +890,9 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -869,9 +906,9 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -885,39 +922,39 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="26">
         <v>0.5</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="26">
         <v>0.5</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="21">
+        <v>16</v>
+      </c>
+      <c r="D14" s="22">
         <f>SUM(D6:D13)</f>
         <v>3.25</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="23">
         <f>SUM(E6:E13)</f>
         <v>4.5</v>
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -925,7 +962,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -933,20 +970,20 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="23">
+        <v>18</v>
+      </c>
+      <c r="E17" s="20">
         <f>SUM(D14+E14)</f>
         <v>7.75</v>
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -954,7 +991,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -962,7 +999,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -970,7 +1007,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -978,7 +1015,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -986,7 +1023,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -994,7 +1031,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1002,7 +1039,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1010,7 +1047,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1018,7 +1055,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1026,7 +1063,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1034,7 +1071,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1042,7 +1079,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1050,7 +1087,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>